<commit_message>
Created Search Functionality and related objects test suite collection
</commit_message>
<xml_diff>
--- a/Data Files/ExcelData.xlsx
+++ b/Data Files/ExcelData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tezza\git\Masoko\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876ACBB7-67C7-4896-8316-4DC0C30AED9F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D783DD5-270C-4624-A08B-1558A60609CB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7320" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -95,9 +95,6 @@
     <t>url</t>
   </si>
   <si>
-    <t>Verification Message</t>
-  </si>
-  <si>
     <t>https://www.masoko.com/</t>
   </si>
   <si>
@@ -113,13 +110,16 @@
     <t>Invalid login or password.</t>
   </si>
   <si>
-    <t>Lewis Mocha</t>
-  </si>
-  <si>
     <t>Please enter a valid email address</t>
   </si>
   <si>
     <t>sfdwgdbsg</t>
+  </si>
+  <si>
+    <t>VerificationMessage</t>
+  </si>
+  <si>
+    <t>My Account</t>
   </si>
 </sst>
 </file>
@@ -507,7 +507,7 @@
         <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -585,7 +585,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,18 +607,18 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -626,21 +626,21 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
         <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -648,10 +648,10 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
         <v>26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -662,7 +662,7 @@
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>